<commit_message>
Project 1 code till Sep 4th
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/excels/MasterTestData.xlsx
+++ b/target/test-classes/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\010LivetechWS\AdactinHybridFramework\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC855BD5-5681-4D1E-AF1C-67B73126FCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72213FAB-BF30-4F49-AE3B-E51321070D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0553831A-864E-45A9-94AF-A275648CAEA8}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.2" x14ac:dyDescent="0.6"/>

</xml_diff>